<commit_message>
* DOC-99 Added sites and site groups topics. * Tweaked mkbp tool and associated files. Convereted to json input.
</commit_message>
<xml_diff>
--- a/_tools/mkbp/pbar-E90host.xlsx
+++ b/_tools/mkbp/pbar-E90host.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="pbar-E90host" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="59">
   <si>
     <t>menu1</t>
   </si>
@@ -181,9 +181,6 @@
   </si>
   <si>
     <t>Config Manager</t>
-  </si>
-  <si>
-    <t>OnDemand</t>
   </si>
   <si>
     <t>About</t>
@@ -1005,10 +1002,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L49"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L48" sqref="L48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1039,16 +1036,16 @@
         <v>7</v>
       </c>
       <c r="I1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
         <v>56</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>57</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>58</v>
-      </c>
-      <c r="L1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -1110,19 +1107,19 @@
         <v>783</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I49" si="0">IF(C3="","",C3/G3*100)</f>
+        <f t="shared" ref="I3:I48" si="0">IF(C3="","",C3/G3*100)</f>
         <v>0.44150110375275936</v>
       </c>
       <c r="J3">
-        <f t="shared" ref="J3:J49" si="1">IF(D3="","",D3/H3*100)</f>
+        <f t="shared" ref="J3:J48" si="1">IF(D3="","",D3/H3*100)</f>
         <v>3.1928480204342273</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K49" si="2">IF(E3="","",E3/G3*100)</f>
+        <f t="shared" ref="K3:K48" si="2">IF(E3="","",E3/G3*100)</f>
         <v>18.322295805739515</v>
       </c>
       <c r="L3">
-        <f t="shared" ref="L3:L49" si="3">IF(F3="","",F3/H3*100)</f>
+        <f t="shared" ref="L3:L48" si="3">IF(F3="","",F3/H3*100)</f>
         <v>0</v>
       </c>
     </row>
@@ -2969,48 +2966,6 @@
       <c r="L48">
         <f t="shared" si="3"/>
         <v>79.054916985951479</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>39</v>
-      </c>
-      <c r="B49" t="s">
-        <v>55</v>
-      </c>
-      <c r="C49">
-        <v>2</v>
-      </c>
-      <c r="D49">
-        <v>350</v>
-      </c>
-      <c r="E49">
-        <v>247</v>
-      </c>
-      <c r="F49">
-        <v>656</v>
-      </c>
-      <c r="G49">
-        <v>453</v>
-      </c>
-      <c r="H49">
-        <v>783</v>
-      </c>
-      <c r="I49">
-        <f t="shared" si="0"/>
-        <v>0.44150110375275936</v>
-      </c>
-      <c r="J49">
-        <f t="shared" si="1"/>
-        <v>44.699872286079184</v>
-      </c>
-      <c r="K49">
-        <f t="shared" si="2"/>
-        <v>54.525386313465788</v>
-      </c>
-      <c r="L49">
-        <f t="shared" si="3"/>
-        <v>83.780332056194126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>